<commit_message>
added html file names for each line in configuration file
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="73">
   <si>
     <t>input_xlsx</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>"15=IGBT + Diode"</t>
+  </si>
+  <si>
+    <t>output_html</t>
+  </si>
+  <si>
+    <t>MOSFET.html</t>
+  </si>
+  <si>
+    <t>IGBT_modules.html</t>
+  </si>
+  <si>
+    <t>IGBT_Discretes.html</t>
   </si>
 </sst>
 </file>
@@ -549,25 +561,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="36.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="2" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="36.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -575,37 +587,40 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -613,28 +628,31 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -642,28 +660,31 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -671,28 +692,31 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -700,28 +724,31 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -729,28 +756,31 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -758,28 +788,31 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -787,28 +820,31 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -816,28 +852,31 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -845,28 +884,31 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -874,28 +916,31 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -903,28 +948,31 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -932,28 +980,31 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>28</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -961,28 +1012,31 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -990,28 +1044,31 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>29</v>
       </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="I15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="L15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1019,28 +1076,31 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>28</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="I16" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1048,28 +1108,31 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>25</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="I17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1077,28 +1140,31 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>29</v>
       </c>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="I18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="L18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1106,28 +1172,31 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
         <v>35</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>28</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>30</v>
       </c>
-      <c r="H19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="I19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="L19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1135,28 +1204,31 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>21</v>
       </c>
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="I20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1164,28 +1236,31 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
         <v>37</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>26</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="I21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1193,28 +1268,31 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
         <v>37</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>28</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>30</v>
       </c>
-      <c r="H22" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="I22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="L22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1222,28 +1300,31 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
         <v>47</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>21</v>
       </c>
-      <c r="H23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1251,28 +1332,31 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>26</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>29</v>
       </c>
-      <c r="H24" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="L24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1280,28 +1364,31 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
         <v>47</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>28</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>30</v>
       </c>
-      <c r="H25" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1309,25 +1396,28 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>58</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>50</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>49</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>52</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>51</v>
       </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1335,28 +1425,31 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>58</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>54</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>49</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>52</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>51</v>
       </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="M27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1364,25 +1457,28 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
         <v>58</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>55</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>28</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>57</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>56</v>
       </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1390,28 +1486,31 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
         <v>60</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>61</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>28</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>64</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>65</v>
       </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="L29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1419,28 +1518,31 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
         <v>60</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>63</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>67</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>65</v>
       </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="L30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1448,28 +1550,31 @@
         <v>59</v>
       </c>
       <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
         <v>60</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>62</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>28</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>64</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>65</v>
       </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1477,24 +1582,27 @@
         <v>59</v>
       </c>
       <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
         <v>60</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>62</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>63</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>67</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>65</v>
       </c>
-      <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
style change to infineon standards
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="125">
   <si>
     <t>input_xlsx</t>
   </si>
@@ -162,9 +162,6 @@
     <t>15=Automotive</t>
   </si>
   <si>
-    <t>All Dual IGBT Modules</t>
-  </si>
-  <si>
     <t>9 8 10 11 12 14 15 7 3</t>
   </si>
   <si>
@@ -298,6 +295,111 @@
   </si>
   <si>
     <t>4 5 6 7 8 9 10 11 17 18 12 13 14 15 16 3 19 20 21</t>
+  </si>
+  <si>
+    <t>"8=Dual"</t>
+  </si>
+  <si>
+    <t>"8=Single switch"</t>
+  </si>
+  <si>
+    <t>6 12 11 17 1</t>
+  </si>
+  <si>
+    <t>Voltage, Housing</t>
+  </si>
+  <si>
+    <t>6 17 11 1</t>
+  </si>
+  <si>
+    <t>Dual (Half-Bridge)</t>
+  </si>
+  <si>
+    <t>Single IGBT</t>
+  </si>
+  <si>
+    <t>Thyristor_Diode_Modules.xlsx</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>3 6 7  5 1</t>
+  </si>
+  <si>
+    <t>3 4 5 6 7 8 9 10 11</t>
+  </si>
+  <si>
+    <t>Diodes &amp; Thyristors</t>
+  </si>
+  <si>
+    <t>Gate_drivers.html</t>
+  </si>
+  <si>
+    <t>Gate_Driver_Ics.xlsx</t>
+  </si>
+  <si>
+    <t>Gate Drivers</t>
+  </si>
+  <si>
+    <t>For IGBT</t>
+  </si>
+  <si>
+    <t>For MOSFET</t>
+  </si>
+  <si>
+    <t>For SiC</t>
+  </si>
+  <si>
+    <t>For GaN</t>
+  </si>
+  <si>
+    <t>Voltage, Output Current</t>
+  </si>
+  <si>
+    <t>5 6 10 16 1</t>
+  </si>
+  <si>
+    <t>4 5 6 11 12 13 14 15 16 35</t>
+  </si>
+  <si>
+    <t>"15=IGBT"</t>
+  </si>
+  <si>
+    <t>"15=MOSFET"</t>
+  </si>
+  <si>
+    <t>"15=SiC"</t>
+  </si>
+  <si>
+    <t>"15=GaN"</t>
+  </si>
+  <si>
+    <t>IPM.xlsx</t>
+  </si>
+  <si>
+    <t>IPM.html</t>
+  </si>
+  <si>
+    <t>IPM</t>
+  </si>
+  <si>
+    <t>Intillegent Power Modules</t>
+  </si>
+  <si>
+    <t>9 12 10 5 1</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 9 10 11 12 13 14</t>
+  </si>
+  <si>
+    <t>9 10 12 5 1</t>
+  </si>
+  <si>
+    <t>Voltage, P&lt;sub&gt;mot&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>9 13 10 12 5 1</t>
   </si>
 </sst>
 </file>
@@ -615,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,10 +745,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -681,22 +783,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -716,22 +818,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
@@ -751,22 +853,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -786,22 +888,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -821,22 +923,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
@@ -856,22 +958,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -891,22 +993,22 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -926,22 +1028,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
@@ -961,22 +1063,22 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
@@ -996,22 +1098,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -1031,22 +1133,22 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -1066,22 +1168,22 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
@@ -1101,22 +1203,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -1136,22 +1238,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
@@ -1171,22 +1273,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
         <v>26</v>
@@ -1206,22 +1308,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -1241,22 +1343,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
         <v>25</v>
@@ -1276,22 +1378,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>
@@ -1311,22 +1413,22 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -1346,22 +1448,22 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
         <v>25</v>
@@ -1381,22 +1483,22 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
@@ -1416,22 +1518,22 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -1451,22 +1553,22 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G24" t="s">
         <v>25</v>
@@ -1486,22 +1588,22 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
         <v>26</v>
@@ -1521,22 +1623,22 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s">
         <v>41</v>
@@ -1553,22 +1655,22 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" t="s">
         <v>41</v>
@@ -1588,275 +1690,721 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="G28" t="s">
         <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K28">
         <v>2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="J29" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="K29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="J30" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="K30">
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J31" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="K31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="G32" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="I32" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="J32" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="K32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="J33" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="K33">
         <v>2</v>
       </c>
-      <c r="N33" t="s">
-        <v>81</v>
+      <c r="M33" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="G34" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I34" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="J34" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="K34">
         <v>2</v>
       </c>
-      <c r="N34" t="s">
-        <v>82</v>
+      <c r="M34" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I35" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" t="s">
+        <v>54</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="M36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="M37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J38" t="s">
+        <v>111</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="N38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I39" t="s">
+        <v>110</v>
+      </c>
+      <c r="J39" t="s">
+        <v>111</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="N39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" t="s">
+        <v>111</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="N40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" t="s">
+        <v>110</v>
+      </c>
+      <c r="J41" t="s">
+        <v>111</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="N41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I42" t="s">
+        <v>79</v>
+      </c>
+      <c r="J42" t="s">
+        <v>75</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="N42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" t="s">
+        <v>41</v>
+      </c>
+      <c r="I43" t="s">
+        <v>79</v>
+      </c>
+      <c r="J43" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="N43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" t="s">
+        <v>100</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
         <v>84</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D45" t="s">
         <v>85</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E45" t="s">
         <v>86</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F45" t="s">
         <v>87</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G45" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" t="s">
         <v>88</v>
       </c>
-      <c r="G35" t="s">
+      <c r="J45" t="s">
+        <v>89</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46" t="s">
+        <v>124</v>
+      </c>
+      <c r="J46" t="s">
+        <v>121</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I47" t="s">
+        <v>120</v>
+      </c>
+      <c r="J47" t="s">
+        <v>121</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" t="s">
         <v>26</v>
       </c>
-      <c r="I35" t="s">
-        <v>89</v>
-      </c>
-      <c r="J35" t="s">
-        <v>90</v>
-      </c>
-      <c r="K35">
+      <c r="I48" t="s">
+        <v>122</v>
+      </c>
+      <c r="J48" t="s">
+        <v>121</v>
+      </c>
+      <c r="K48">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
visual changes, added datasheet link and product page link
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>All N-Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Automotive N-Type </t>
-  </si>
-  <si>
     <t>All P-Type</t>
   </si>
   <si>
@@ -400,6 +397,9 @@
   </si>
   <si>
     <t>9 13 10 12 5 1</t>
+  </si>
+  <si>
+    <t>Automotive N-Type</t>
   </si>
 </sst>
 </file>
@@ -719,25 +719,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="36.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -781,7 +781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -798,7 +798,7 @@
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -816,7 +816,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -833,7 +833,7 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
@@ -851,7 +851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -868,7 +868,7 @@
         <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -886,7 +886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -900,10 +900,10 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -921,7 +921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -935,10 +935,10 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
@@ -956,7 +956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -970,10 +970,10 @@
         <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -991,7 +991,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -1026,7 +1026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
@@ -1061,7 +1061,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
         <v>26</v>
@@ -1096,7 +1096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1110,10 +1110,10 @@
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -1131,7 +1131,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1145,10 +1145,10 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -1166,7 +1166,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1180,10 +1180,10 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
         <v>26</v>
@@ -1201,7 +1201,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
@@ -1236,7 +1236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
@@ -1271,7 +1271,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
         <v>26</v>
@@ -1306,7 +1306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1320,10 +1320,10 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -1341,7 +1341,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1355,10 +1355,10 @@
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" t="s">
         <v>25</v>
@@ -1376,7 +1376,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1390,10 +1390,10 @@
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>
@@ -1411,7 +1411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1425,10 +1425,10 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
@@ -1446,7 +1446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1460,10 +1460,10 @@
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s">
         <v>25</v>
@@ -1481,7 +1481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1495,10 +1495,10 @@
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
@@ -1516,7 +1516,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1530,10 +1530,10 @@
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -1551,7 +1551,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1565,10 +1565,10 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
         <v>25</v>
@@ -1586,7 +1586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1600,10 +1600,10 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" t="s">
         <v>26</v>
@@ -1621,7 +1621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F26" t="s">
         <v>47</v>
@@ -1653,7 +1653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
         <v>47</v>
@@ -1688,7 +1688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1702,10 +1702,10 @@
         <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G28" t="s">
         <v>26</v>
@@ -1720,10 +1720,10 @@
         <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1737,16 +1737,16 @@
         <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" t="s">
         <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J29" t="s">
         <v>45</v>
@@ -1755,10 +1755,10 @@
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1772,16 +1772,16 @@
         <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G30" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" t="s">
         <v>93</v>
-      </c>
-      <c r="I30" t="s">
-        <v>94</v>
       </c>
       <c r="J30" t="s">
         <v>45</v>
@@ -1790,10 +1790,10 @@
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1807,10 +1807,10 @@
         <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
@@ -1825,10 +1825,10 @@
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1842,16 +1842,16 @@
         <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
         <v>25</v>
       </c>
       <c r="I32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" t="s">
         <v>45</v>
@@ -1860,10 +1860,10 @@
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1877,16 +1877,16 @@
         <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" t="s">
         <v>93</v>
-      </c>
-      <c r="I33" t="s">
-        <v>94</v>
       </c>
       <c r="J33" t="s">
         <v>45</v>
@@ -1895,115 +1895,106 @@
         <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="F34" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="I34" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="J34" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="K34">
         <v>2</v>
       </c>
-      <c r="M34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="G35" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I35" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="J35" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="K35">
         <v>2</v>
       </c>
-      <c r="M35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="G36" t="s">
         <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="J36" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="K36">
         <v>2</v>
       </c>
-      <c r="M36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2020,13 +2011,13 @@
         <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G37" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J37" t="s">
         <v>54</v>
@@ -2035,374 +2026,383 @@
         <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="I38" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="J38" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="K38">
         <v>2</v>
       </c>
-      <c r="N38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="G39" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="I39" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="J39" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="K39">
         <v>2</v>
       </c>
-      <c r="N39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="G40" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="I40" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="J40" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="K40">
         <v>2</v>
       </c>
-      <c r="N40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
         <v>103</v>
       </c>
-      <c r="C41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" t="s">
         <v>104</v>
       </c>
-      <c r="E41" t="s">
-        <v>104</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>108</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>109</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>110</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="N41" t="s">
         <v>111</v>
       </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-      <c r="N41" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="F42" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="I42" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="J42" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="K42">
         <v>2</v>
       </c>
       <c r="N42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="F43" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="G43" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="I43" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="J43" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="K43">
         <v>2</v>
       </c>
       <c r="N43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G44" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="I44" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="J44" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F45" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G45" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I45" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="J45" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="K45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E46" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="F46" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="G46" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="I46" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="J46" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="K46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F47" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="G47" t="s">
         <v>41</v>
       </c>
       <c r="I47" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="J47" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="K47">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="F48" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="G48" t="s">
         <v>26</v>
       </c>
       <c r="I48" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="J48" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -2422,59 +2422,59 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
preparation to merge projects to one SPSM_BUILDER
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="185">
   <si>
     <t>input_xlsx</t>
   </si>
@@ -565,6 +565,21 @@
   </si>
   <si>
     <t>20=Automotive; 9=N; "10=12 V, 20 V, 24 V, 25 V, 30 V, 34 V, 40 V, 55 V, 60 V, 75 V, 80 V"</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>"8=Sixpack"</t>
+  </si>
+  <si>
+    <t>Sixpack</t>
+  </si>
+  <si>
+    <t>"8=PIM"</t>
+  </si>
+  <si>
+    <t>All Configurations</t>
   </si>
 </sst>
 </file>
@@ -882,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1881,7 +1896,7 @@
         <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
       <c r="H26" t="s">
         <v>35</v>
@@ -1916,7 +1931,7 @@
         <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
       <c r="H27" t="s">
         <v>35</v>
@@ -2167,34 +2182,37 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="J34" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="K34" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="L34">
         <v>2</v>
+      </c>
+      <c r="N34" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -2202,34 +2220,37 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="F35" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="G35" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="K35" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="L35">
         <v>2</v>
+      </c>
+      <c r="N35" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -2237,34 +2258,37 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="G36" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="H36" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="J36" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="K36" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="L36">
         <v>2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -2272,37 +2296,37 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F37" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G37" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="H37" t="s">
         <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="K37" t="s">
-        <v>118</v>
-      </c>
-      <c r="L37" t="s">
-        <v>120</v>
-      </c>
-      <c r="N37" t="s">
-        <v>116</v>
+        <v>39</v>
+      </c>
+      <c r="L37">
+        <v>2</v>
+      </c>
+      <c r="O37" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2310,37 +2334,37 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F38" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G38" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="H38" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="K38" t="s">
-        <v>118</v>
-      </c>
-      <c r="L38" t="s">
-        <v>120</v>
-      </c>
-      <c r="N38" t="s">
-        <v>116</v>
+        <v>39</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="O38" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -2348,37 +2372,37 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F39" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G39" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="H39" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="J39" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="K39" t="s">
-        <v>118</v>
-      </c>
-      <c r="L39" t="s">
-        <v>120</v>
-      </c>
-      <c r="N39" t="s">
-        <v>117</v>
+        <v>39</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="O39" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -2386,37 +2410,34 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="G40" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="H40" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="J40" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="K40" t="s">
-        <v>118</v>
-      </c>
-      <c r="L40" t="s">
-        <v>120</v>
-      </c>
-      <c r="N40" t="s">
-        <v>117</v>
+        <v>93</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -2424,37 +2445,34 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="H41" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="J41" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="K41" t="s">
-        <v>113</v>
-      </c>
-      <c r="L41" t="s">
-        <v>120</v>
-      </c>
-      <c r="O41" t="s">
-        <v>109</v>
+        <v>93</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -2462,37 +2480,34 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F42" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H42" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="J42" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K42" t="s">
-        <v>113</v>
-      </c>
-      <c r="L42" t="s">
-        <v>120</v>
-      </c>
-      <c r="O42" t="s">
-        <v>110</v>
+        <v>93</v>
+      </c>
+      <c r="L42">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -2500,37 +2515,37 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="G43" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="J43" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K43" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L43" t="s">
         <v>120</v>
       </c>
-      <c r="O43" t="s">
-        <v>111</v>
+      <c r="N43" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -2538,37 +2553,37 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="H44" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="J44" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K44" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="L44" t="s">
         <v>120</v>
       </c>
-      <c r="O44" t="s">
-        <v>112</v>
+      <c r="N44" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -2576,37 +2591,37 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E45" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G45" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H45" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J45" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="K45" t="s">
-        <v>63</v>
-      </c>
-      <c r="L45">
-        <v>2</v>
-      </c>
-      <c r="O45" t="s">
-        <v>68</v>
+        <v>118</v>
+      </c>
+      <c r="L45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N45" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -2614,37 +2629,37 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="F46" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G46" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="H46" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="J46" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="K46" t="s">
-        <v>63</v>
-      </c>
-      <c r="L46">
-        <v>2</v>
-      </c>
-      <c r="O46" t="s">
-        <v>69</v>
+        <v>118</v>
+      </c>
+      <c r="L46" t="s">
+        <v>120</v>
+      </c>
+      <c r="N46" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -2652,34 +2667,37 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F47" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G47" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H47" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="J47" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="K47" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="L47" t="s">
         <v>120</v>
+      </c>
+      <c r="O47" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -2687,37 +2705,37 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="F48" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="G48" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="J48" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="K48" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="L48" t="s">
         <v>120</v>
       </c>
       <c r="O48" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -2725,37 +2743,37 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="F49" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="G49" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="H49" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="J49" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="K49" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="L49" t="s">
         <v>120</v>
       </c>
       <c r="O49" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,28 +2781,37 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="E50" t="s">
-        <v>140</v>
+        <v>82</v>
+      </c>
+      <c r="F50" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" t="s">
+        <v>86</v>
       </c>
       <c r="H50" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="J50" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="K50" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="L50" t="s">
         <v>120</v>
+      </c>
+      <c r="O50" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -2792,28 +2819,37 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>62</v>
+      </c>
+      <c r="F51" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" t="s">
+        <v>64</v>
       </c>
       <c r="H51" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="J51" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="K51" t="s">
-        <v>147</v>
-      </c>
-      <c r="L51" t="s">
-        <v>120</v>
+        <v>63</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="O51" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -2821,28 +2857,37 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="D52" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>62</v>
+      </c>
+      <c r="F52" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" t="s">
+        <v>66</v>
       </c>
       <c r="H52" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="J52" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="K52" t="s">
-        <v>155</v>
-      </c>
-      <c r="L52" t="s">
-        <v>120</v>
+        <v>63</v>
+      </c>
+      <c r="L52">
+        <v>2</v>
+      </c>
+      <c r="O52" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -2850,25 +2895,31 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="D53" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>159</v>
+        <v>62</v>
+      </c>
+      <c r="F53" t="s">
+        <v>78</v>
+      </c>
+      <c r="G53" t="s">
+        <v>79</v>
       </c>
       <c r="H53" t="s">
-        <v>160</v>
+        <v>35</v>
       </c>
       <c r="J53" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="K53" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s">
         <v>120</v>
@@ -2879,28 +2930,37 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>163</v>
+        <v>126</v>
+      </c>
+      <c r="F54" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" t="s">
+        <v>127</v>
       </c>
       <c r="H54" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="J54" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="K54" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="L54" t="s">
         <v>120</v>
+      </c>
+      <c r="O54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -2908,27 +2968,210 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" t="s">
+        <v>129</v>
+      </c>
+      <c r="G55" t="s">
+        <v>127</v>
+      </c>
+      <c r="H55" t="s">
+        <v>130</v>
+      </c>
+      <c r="J55" t="s">
+        <v>131</v>
+      </c>
+      <c r="K55" t="s">
+        <v>132</v>
+      </c>
+      <c r="L55" t="s">
+        <v>120</v>
+      </c>
+      <c r="O55" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
+        <v>138</v>
+      </c>
+      <c r="E56" t="s">
+        <v>140</v>
+      </c>
+      <c r="H56" t="s">
+        <v>139</v>
+      </c>
+      <c r="J56" t="s">
+        <v>142</v>
+      </c>
+      <c r="K56" t="s">
+        <v>141</v>
+      </c>
+      <c r="L56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" t="s">
+        <v>145</v>
+      </c>
+      <c r="E57" t="s">
+        <v>146</v>
+      </c>
+      <c r="H57" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" t="s">
+        <v>148</v>
+      </c>
+      <c r="K57" t="s">
+        <v>147</v>
+      </c>
+      <c r="L57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" t="s">
+        <v>152</v>
+      </c>
+      <c r="H58" t="s">
+        <v>153</v>
+      </c>
+      <c r="J58" t="s">
+        <v>154</v>
+      </c>
+      <c r="K58" t="s">
+        <v>155</v>
+      </c>
+      <c r="L58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" t="s">
+        <v>159</v>
+      </c>
+      <c r="H59" t="s">
+        <v>160</v>
+      </c>
+      <c r="J59" t="s">
+        <v>161</v>
+      </c>
+      <c r="K59" t="s">
+        <v>162</v>
+      </c>
+      <c r="L59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" t="s">
+        <v>176</v>
+      </c>
+      <c r="E60" t="s">
+        <v>163</v>
+      </c>
+      <c r="H60" t="s">
+        <v>166</v>
+      </c>
+      <c r="J60" t="s">
+        <v>167</v>
+      </c>
+      <c r="K60" t="s">
+        <v>168</v>
+      </c>
+      <c r="L60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
         <v>170</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C61" t="s">
         <v>169</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D61" t="s">
         <v>175</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E61" t="s">
         <v>171</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H61" t="s">
         <v>172</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J61" t="s">
         <v>173</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K61" t="s">
         <v>174</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L61" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>